<commit_message>
Updated Sprint 2 Test result
Distance Test between Dundee and Glasgow
</commit_message>
<xml_diff>
--- a/Sprint 2/Sprint_Backlog/Sprint2TestPlan.xlsx
+++ b/Sprint 2/Sprint_Backlog/Sprint2TestPlan.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afzalmiah\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3360674-5888-42A9-BFAF-D9364F573E7F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agile Test Plan" sheetId="1" r:id="rId1"/>
@@ -20,14 +21,6 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -36,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="79">
   <si>
     <t>TESTER COMMENTS</t>
   </si>
@@ -264,12 +257,21 @@
   </si>
   <si>
     <t>Need to scale down</t>
+  </si>
+  <si>
+    <t>Correct distance between Dundee and Glasgow</t>
+  </si>
+  <si>
+    <t>Calculate Distance between Dundee and Glasgow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Henry </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -564,7 +566,7 @@
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="5"/>
+    <cellStyle name="Normal 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
   <dxfs count="35">
     <dxf>
@@ -1041,7 +1043,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp19.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="'-Disclaimer-'!$A$19" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="'-Disclaimer-'!$A$19" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1101,7 +1103,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp32.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="'-Disclaimer-'!$A$19" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="'-Disclaimer-'!$A$19" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1125,7 +1127,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="'-Disclaimer-'!$A$19" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="'-Disclaimer-'!$A$19" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3598,16 +3600,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-4.9989318521683403E-2"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:Y76"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
+      <selection pane="bottomLeft" activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -4604,13 +4606,25 @@
       <c r="B27" s="14">
         <v>43284</v>
       </c>
-      <c r="C27" s="25"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
+      <c r="C27" s="25">
+        <v>2</v>
+      </c>
+      <c r="D27" s="15">
+        <v>2</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="G27" s="15" t="s">
+        <v>58</v>
+      </c>
       <c r="H27" s="16"/>
-      <c r="I27" s="15"/>
+      <c r="I27" s="15" t="s">
+        <v>78</v>
+      </c>
       <c r="J27" s="15"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
@@ -5933,7 +5947,7 @@
     <mergeCell ref="B40:J40"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B40:J40" r:id="rId1" display="CLICK HERE TO CREATE IN SMARTSHEET"/>
+    <hyperlink ref="B40:J40" r:id="rId1" display="CLICK HERE TO CREATE IN SMARTSHEET" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>
   <pageSetup scale="50" fitToHeight="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
@@ -7292,7 +7306,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
@@ -7356,7 +7370,7 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
@@ -7396,15 +7410,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001E699AB3B5B90B4E9587B6CE8A7722F9" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="327bf17b6c8b56faa046bfad41848f88">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2908a239-9a9c-424d-a25e-b52b320ef348" xmlns:ns4="14699dbd-23eb-47d5-a11a-8dab2a8bfb64" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dfb120bc1534939806b9bc4170ddcf21" ns3:_="" ns4:_="">
     <xsd:import namespace="2908a239-9a9c-424d-a25e-b52b320ef348"/>
@@ -7575,6 +7580,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -7582,14 +7596,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73B01F70-A4AC-4F1F-BFEA-2CE3694CCB74}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{395500BF-5D64-47FA-8516-846D2479598F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7604,6 +7610,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73B01F70-A4AC-4F1F-BFEA-2CE3694CCB74}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>